<commit_message>
Replaced deleted video :/
</commit_message>
<xml_diff>
--- a/MewPipe.DataFeeder/datas/videos.xlsx
+++ b/MewPipe.DataFeeder/datas/videos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Documents\projets\4PJT\4pjt_mewpipe\MewPipe.DataFeeder\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Documents\projets\4PJT\4pjt_mewpipe\MewPipe.DataFeeder\datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -176,9 +176,6 @@
     <t>https://www.youtube.com/watch?v=kzpTFrWJ4MA</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=K2E6lH7yD2Q</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=AF_HUYEwYVc</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=fukpMH8Cx_g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=uYosBJr-fMI</t>
   </si>
 </sst>
 </file>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
         <v>34</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
         <v>34</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
         <v>34</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
         <v>34</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
         <v>34</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
         <v>34</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
         <v>34</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
         <v>34</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>34</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>34</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>34</v>
@@ -1157,242 +1157,242 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1409,78 +1409,77 @@
     <hyperlink ref="A35" r:id="rId10"/>
     <hyperlink ref="A38" r:id="rId11"/>
     <hyperlink ref="A41" r:id="rId12"/>
-    <hyperlink ref="A49" r:id="rId13"/>
-    <hyperlink ref="A51" r:id="rId14"/>
-    <hyperlink ref="A55" r:id="rId15"/>
-    <hyperlink ref="A57" r:id="rId16"/>
-    <hyperlink ref="A60" r:id="rId17"/>
-    <hyperlink ref="A64" r:id="rId18"/>
-    <hyperlink ref="A69" r:id="rId19"/>
-    <hyperlink ref="A73" r:id="rId20"/>
-    <hyperlink ref="A88" r:id="rId21"/>
-    <hyperlink ref="A89" r:id="rId22"/>
-    <hyperlink ref="A2" r:id="rId23"/>
-    <hyperlink ref="A3" r:id="rId24"/>
-    <hyperlink ref="A5" r:id="rId25"/>
-    <hyperlink ref="A8" r:id="rId26"/>
-    <hyperlink ref="A9" r:id="rId27"/>
-    <hyperlink ref="A14" r:id="rId28"/>
-    <hyperlink ref="A15" r:id="rId29"/>
-    <hyperlink ref="A17" r:id="rId30"/>
-    <hyperlink ref="A19" r:id="rId31"/>
-    <hyperlink ref="A20" r:id="rId32"/>
-    <hyperlink ref="A21" r:id="rId33"/>
-    <hyperlink ref="A22" r:id="rId34"/>
-    <hyperlink ref="A24" r:id="rId35"/>
-    <hyperlink ref="A26" r:id="rId36"/>
-    <hyperlink ref="A27" r:id="rId37"/>
-    <hyperlink ref="A28" r:id="rId38"/>
-    <hyperlink ref="A32" r:id="rId39"/>
-    <hyperlink ref="A31" r:id="rId40"/>
-    <hyperlink ref="A33" r:id="rId41"/>
-    <hyperlink ref="A34" r:id="rId42"/>
-    <hyperlink ref="A36" r:id="rId43"/>
-    <hyperlink ref="A37" r:id="rId44"/>
-    <hyperlink ref="A39" r:id="rId45"/>
-    <hyperlink ref="A40" r:id="rId46"/>
-    <hyperlink ref="A42" r:id="rId47"/>
-    <hyperlink ref="A43" r:id="rId48"/>
-    <hyperlink ref="A44" r:id="rId49"/>
-    <hyperlink ref="A45" r:id="rId50"/>
-    <hyperlink ref="A46" r:id="rId51"/>
-    <hyperlink ref="A47" r:id="rId52"/>
-    <hyperlink ref="A48" r:id="rId53"/>
-    <hyperlink ref="A50" r:id="rId54"/>
-    <hyperlink ref="A52" r:id="rId55"/>
-    <hyperlink ref="A53" r:id="rId56"/>
-    <hyperlink ref="A54" r:id="rId57"/>
-    <hyperlink ref="A56" r:id="rId58"/>
-    <hyperlink ref="A58" r:id="rId59"/>
-    <hyperlink ref="A59" r:id="rId60"/>
-    <hyperlink ref="A61" r:id="rId61"/>
-    <hyperlink ref="A62" r:id="rId62"/>
-    <hyperlink ref="A63" r:id="rId63"/>
-    <hyperlink ref="A65" r:id="rId64"/>
-    <hyperlink ref="A66" r:id="rId65"/>
-    <hyperlink ref="A67" r:id="rId66"/>
-    <hyperlink ref="A68" r:id="rId67"/>
-    <hyperlink ref="A70" r:id="rId68"/>
-    <hyperlink ref="A71" r:id="rId69"/>
-    <hyperlink ref="A72" r:id="rId70"/>
-    <hyperlink ref="A74" r:id="rId71"/>
-    <hyperlink ref="A75" r:id="rId72"/>
-    <hyperlink ref="A76" r:id="rId73"/>
-    <hyperlink ref="A77" r:id="rId74"/>
-    <hyperlink ref="A78" r:id="rId75"/>
-    <hyperlink ref="A79" r:id="rId76"/>
-    <hyperlink ref="A80" r:id="rId77"/>
-    <hyperlink ref="A81" r:id="rId78"/>
-    <hyperlink ref="A82" r:id="rId79"/>
-    <hyperlink ref="A83" r:id="rId80"/>
-    <hyperlink ref="A84" r:id="rId81"/>
-    <hyperlink ref="A85" r:id="rId82"/>
-    <hyperlink ref="A86" r:id="rId83"/>
-    <hyperlink ref="A87" r:id="rId84"/>
+    <hyperlink ref="A51" r:id="rId13"/>
+    <hyperlink ref="A55" r:id="rId14"/>
+    <hyperlink ref="A57" r:id="rId15"/>
+    <hyperlink ref="A60" r:id="rId16"/>
+    <hyperlink ref="A64" r:id="rId17"/>
+    <hyperlink ref="A69" r:id="rId18"/>
+    <hyperlink ref="A73" r:id="rId19"/>
+    <hyperlink ref="A88" r:id="rId20"/>
+    <hyperlink ref="A89" r:id="rId21"/>
+    <hyperlink ref="A2" r:id="rId22"/>
+    <hyperlink ref="A3" r:id="rId23"/>
+    <hyperlink ref="A5" r:id="rId24"/>
+    <hyperlink ref="A8" r:id="rId25"/>
+    <hyperlink ref="A9" r:id="rId26"/>
+    <hyperlink ref="A14" r:id="rId27"/>
+    <hyperlink ref="A15" r:id="rId28"/>
+    <hyperlink ref="A17" r:id="rId29"/>
+    <hyperlink ref="A19" r:id="rId30"/>
+    <hyperlink ref="A20" r:id="rId31"/>
+    <hyperlink ref="A21" r:id="rId32"/>
+    <hyperlink ref="A22" r:id="rId33"/>
+    <hyperlink ref="A24" r:id="rId34"/>
+    <hyperlink ref="A26" r:id="rId35"/>
+    <hyperlink ref="A27" r:id="rId36"/>
+    <hyperlink ref="A28" r:id="rId37"/>
+    <hyperlink ref="A32" r:id="rId38"/>
+    <hyperlink ref="A31" r:id="rId39"/>
+    <hyperlink ref="A33" r:id="rId40"/>
+    <hyperlink ref="A34" r:id="rId41"/>
+    <hyperlink ref="A36" r:id="rId42"/>
+    <hyperlink ref="A37" r:id="rId43"/>
+    <hyperlink ref="A39" r:id="rId44"/>
+    <hyperlink ref="A40" r:id="rId45"/>
+    <hyperlink ref="A42" r:id="rId46"/>
+    <hyperlink ref="A43" r:id="rId47"/>
+    <hyperlink ref="A44" r:id="rId48"/>
+    <hyperlink ref="A45" r:id="rId49"/>
+    <hyperlink ref="A46" r:id="rId50"/>
+    <hyperlink ref="A47" r:id="rId51"/>
+    <hyperlink ref="A48" r:id="rId52"/>
+    <hyperlink ref="A50" r:id="rId53"/>
+    <hyperlink ref="A52" r:id="rId54"/>
+    <hyperlink ref="A53" r:id="rId55"/>
+    <hyperlink ref="A54" r:id="rId56"/>
+    <hyperlink ref="A56" r:id="rId57"/>
+    <hyperlink ref="A58" r:id="rId58"/>
+    <hyperlink ref="A59" r:id="rId59"/>
+    <hyperlink ref="A61" r:id="rId60"/>
+    <hyperlink ref="A62" r:id="rId61"/>
+    <hyperlink ref="A63" r:id="rId62"/>
+    <hyperlink ref="A65" r:id="rId63"/>
+    <hyperlink ref="A66" r:id="rId64"/>
+    <hyperlink ref="A67" r:id="rId65"/>
+    <hyperlink ref="A68" r:id="rId66"/>
+    <hyperlink ref="A70" r:id="rId67"/>
+    <hyperlink ref="A71" r:id="rId68"/>
+    <hyperlink ref="A72" r:id="rId69"/>
+    <hyperlink ref="A74" r:id="rId70"/>
+    <hyperlink ref="A75" r:id="rId71"/>
+    <hyperlink ref="A76" r:id="rId72"/>
+    <hyperlink ref="A77" r:id="rId73"/>
+    <hyperlink ref="A78" r:id="rId74"/>
+    <hyperlink ref="A79" r:id="rId75"/>
+    <hyperlink ref="A80" r:id="rId76"/>
+    <hyperlink ref="A81" r:id="rId77"/>
+    <hyperlink ref="A82" r:id="rId78"/>
+    <hyperlink ref="A83" r:id="rId79"/>
+    <hyperlink ref="A84" r:id="rId80"/>
+    <hyperlink ref="A85" r:id="rId81"/>
+    <hyperlink ref="A86" r:id="rId82"/>
+    <hyperlink ref="A87" r:id="rId83"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added "Author" column in videos.xlsx
</commit_message>
<xml_diff>
--- a/MewPipe.DataFeeder/datas/videos.xlsx
+++ b/MewPipe.DataFeeder/datas/videos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
   <si>
     <t>URL</t>
   </si>
@@ -303,13 +303,16 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=uYosBJr-fMI</t>
+  </si>
+  <si>
+    <t>Author</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,13 +328,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -343,15 +367,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -655,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,15 +696,18 @@
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -683,7 +715,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -691,7 +723,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -699,7 +731,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -707,7 +739,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -715,7 +747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -723,7 +755,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -731,7 +763,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -739,7 +771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -747,7 +779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -755,7 +787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -763,7 +795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -771,7 +803,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -779,7 +811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -787,7 +819,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1482,6 +1514,7 @@
     <hyperlink ref="A87" r:id="rId83"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId84"/>
 </worksheet>
 </file>
 

</xml_diff>